<commit_message>
Added tests for vunits.constants
</commit_message>
<xml_diff>
--- a/vunits/tests/test_constants.xlsx
+++ b/vunits/tests/test_constants.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox (Personal)\UDel Documents (Dropbox)\UDel Research\Github\vunits\vunits\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8405F53B-FFD0-4353-8531-144A58F57323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A7EE75-99E1-4FD7-9539-EDAF560C9038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AA336A12-CD5D-469F-9132-8EBAE81227A9}"/>
+    <workbookView minimized="1" xWindow="25320" yWindow="1380" windowWidth="21600" windowHeight="11388" activeTab="1" xr2:uid="{AA336A12-CD5D-469F-9132-8EBAE81227A9}"/>
+    <workbookView xWindow="25596" yWindow="1644" windowWidth="21600" windowHeight="11388" activeTab="1" xr2:uid="{AA4D92D5-837E-46A8-8409-770A3ECE788A}"/>
   </bookViews>
   <sheets>
     <sheet name="ans" sheetId="3" r:id="rId1"/>
@@ -20,14 +21,30 @@
     <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="atto_">Units!$C$168</definedName>
+    <definedName name="c_">constants!$C$6</definedName>
     <definedName name="c_cms">constants!#REF!</definedName>
     <definedName name="c_ms">constants!#REF!</definedName>
+    <definedName name="centI_">Units!$C$162</definedName>
+    <definedName name="deca_">Units!$C$160</definedName>
+    <definedName name="deci_">Units!$C$161</definedName>
+    <definedName name="e_">constants!$C$15</definedName>
     <definedName name="e_C">constants!#REF!</definedName>
+    <definedName name="eps_0_">constants!$C$18</definedName>
+    <definedName name="exa_">Units!$C$153</definedName>
+    <definedName name="F_">constants!$C$16</definedName>
+    <definedName name="femto_">Units!$C$167</definedName>
+    <definedName name="G_">constants!$C$17</definedName>
+    <definedName name="giga_">Units!$C$156</definedName>
+    <definedName name="h_">constants!$C$3</definedName>
+    <definedName name="h_bar_">constants!$C$4</definedName>
     <definedName name="h_Ehs">constants!#REF!</definedName>
     <definedName name="h_eVs">constants!#REF!</definedName>
     <definedName name="h_Has">constants!#REF!</definedName>
     <definedName name="h_Js">constants!#REF!</definedName>
     <definedName name="h_kJs">constants!#REF!</definedName>
+    <definedName name="hecto_">Units!$C$159</definedName>
+    <definedName name="kb_">constants!$C$5</definedName>
     <definedName name="kb_calK">constants!#REF!</definedName>
     <definedName name="kb_EhK">constants!#REF!</definedName>
     <definedName name="kb_eVK">constants!#REF!</definedName>
@@ -35,13 +52,24 @@
     <definedName name="kb_JK">constants!#REF!</definedName>
     <definedName name="kb_kcalK">constants!#REF!</definedName>
     <definedName name="kb_kJK">constants!#REF!</definedName>
+    <definedName name="kilo_">Units!$C$158</definedName>
+    <definedName name="m_e_">constants!$C$7</definedName>
     <definedName name="m_e_amu">constants!#REF!</definedName>
     <definedName name="m_e_g">constants!#REF!</definedName>
     <definedName name="m_e_kg">constants!#REF!</definedName>
+    <definedName name="m_n_">constants!$C$9</definedName>
+    <definedName name="m_p_">constants!$C$8</definedName>
     <definedName name="m_p_amu">constants!#REF!</definedName>
     <definedName name="m_p_g">constants!#REF!</definedName>
     <definedName name="m_p_kg">constants!#REF!</definedName>
-    <definedName name="Na_">constants!#REF!</definedName>
+    <definedName name="mega_">Units!$C$157</definedName>
+    <definedName name="micro_">Units!$C$164</definedName>
+    <definedName name="milli_">Units!$C$163</definedName>
+    <definedName name="mu_0_">constants!$C$19</definedName>
+    <definedName name="N0_">constants!$C$13</definedName>
+    <definedName name="Na_">constants!$C$14</definedName>
+    <definedName name="nano_">Units!$C$165</definedName>
+    <definedName name="P0_">constants!$C$10</definedName>
     <definedName name="P0_atm">constants!#REF!</definedName>
     <definedName name="P0_bar">constants!#REF!</definedName>
     <definedName name="P0_kPa">constants!#REF!</definedName>
@@ -50,6 +78,10 @@
     <definedName name="P0_Pa">constants!#REF!</definedName>
     <definedName name="P0_psi">constants!#REF!</definedName>
     <definedName name="P0_Torr">constants!#REF!</definedName>
+    <definedName name="peta_">Units!$C$154</definedName>
+    <definedName name="pico_">Units!$C$166</definedName>
+    <definedName name="R_">constants!$C$2</definedName>
+    <definedName name="r_bohr_">constants!$C$21</definedName>
     <definedName name="R_calmolK">constants!#REF!</definedName>
     <definedName name="R_cm3atmmolK">constants!#REF!</definedName>
     <definedName name="R_cm3kPamolK">constants!#REF!</definedName>
@@ -57,6 +89,7 @@
     <definedName name="R_EhK">constants!#REF!</definedName>
     <definedName name="R_eVK">constants!#REF!</definedName>
     <definedName name="R_HaK">constants!#REF!</definedName>
+    <definedName name="R_inf_">constants!$C$20</definedName>
     <definedName name="R_JmolK">constants!#REF!</definedName>
     <definedName name="R_kcalmolK">constants!#REF!</definedName>
     <definedName name="R_kJmolK">constants!#REF!</definedName>
@@ -66,14 +99,21 @@
     <definedName name="R_LtorrmolK">constants!#REF!</definedName>
     <definedName name="R_m3barmolK">constants!#REF!</definedName>
     <definedName name="R_m3PamolK">constants!#REF!</definedName>
+    <definedName name="T0_">constants!$C$11</definedName>
     <definedName name="T0_C">constants!#REF!</definedName>
     <definedName name="T0_F">constants!#REF!</definedName>
     <definedName name="T0_K">constants!#REF!</definedName>
     <definedName name="T0_R">constants!#REF!</definedName>
+    <definedName name="tera_">Units!$C$155</definedName>
+    <definedName name="V0_">constants!$C$12</definedName>
     <definedName name="V0_cm3">constants!#REF!</definedName>
     <definedName name="V0_L">constants!#REF!</definedName>
     <definedName name="V0_m3">constants!#REF!</definedName>
     <definedName name="V0_ml">constants!#REF!</definedName>
+    <definedName name="yocto_">Units!$C$170</definedName>
+    <definedName name="yotta_">Units!$C$151</definedName>
+    <definedName name="zepto_">Units!$C$169</definedName>
+    <definedName name="zetta_">Units!$C$152</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -91,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="261">
   <si>
     <t>Name</t>
   </si>
@@ -234,57 +274,6 @@
     <t>test_V0</t>
   </si>
   <si>
-    <t>test_convert_unit</t>
-  </si>
-  <si>
-    <t>test_energy_to_freq</t>
-  </si>
-  <si>
-    <t>test_energy_to_temp</t>
-  </si>
-  <si>
-    <t>test_energy_to_wavenumber</t>
-  </si>
-  <si>
-    <t>test_freq_to_energy</t>
-  </si>
-  <si>
-    <t>test_freq_to_temp</t>
-  </si>
-  <si>
-    <t>test_freq_to_wavenumber</t>
-  </si>
-  <si>
-    <t>test_inertia_to_temp</t>
-  </si>
-  <si>
-    <t>test_temp_to_energy</t>
-  </si>
-  <si>
-    <t>test_temp_to_freq</t>
-  </si>
-  <si>
-    <t>test_temp_to_wavenumber</t>
-  </si>
-  <si>
-    <t>test_wavenumber_to_energy</t>
-  </si>
-  <si>
-    <t>test_wavenumber_to_freq</t>
-  </si>
-  <si>
-    <t>test_wavenumber_to_inertia</t>
-  </si>
-  <si>
-    <t>test_wavenumber_to_temp</t>
-  </si>
-  <si>
-    <t>test_debye_to_einstein</t>
-  </si>
-  <si>
-    <t>test_einstein_to_debye</t>
-  </si>
-  <si>
     <t>Energy</t>
   </si>
   <si>
@@ -294,12 +283,6 @@
     <t>Hz</t>
   </si>
   <si>
-    <t>T conversion</t>
-  </si>
-  <si>
-    <t>Unit Conversion</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -384,9 +367,6 @@
     <t>Pressure</t>
   </si>
   <si>
-    <t>bar=True</t>
-  </si>
-  <si>
     <t>sec</t>
   </si>
   <si>
@@ -733,6 +713,207 @@
   </si>
   <si>
     <t>Bohr radius</t>
+  </si>
+  <si>
+    <t>test_h_bar</t>
+  </si>
+  <si>
+    <t>test_m_n</t>
+  </si>
+  <si>
+    <t>test_N0</t>
+  </si>
+  <si>
+    <t>test_Na</t>
+  </si>
+  <si>
+    <t>test_e</t>
+  </si>
+  <si>
+    <t>test_F</t>
+  </si>
+  <si>
+    <t>test_G</t>
+  </si>
+  <si>
+    <t>test_eps_0</t>
+  </si>
+  <si>
+    <t>test_mu_0</t>
+  </si>
+  <si>
+    <t>test_R_inf</t>
+  </si>
+  <si>
+    <t>test_r_bohr</t>
+  </si>
+  <si>
+    <t>kJ/mol/K</t>
+  </si>
+  <si>
+    <t>L atm/mol/K</t>
+  </si>
+  <si>
+    <t>kcal/mol/K</t>
+  </si>
+  <si>
+    <t>yotta</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>zetta</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>exa</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>peta</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>tera</t>
+  </si>
+  <si>
+    <t>giga</t>
+  </si>
+  <si>
+    <t>mega</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>kilo</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>hecto</t>
+  </si>
+  <si>
+    <t>deca</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>deci</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>centi</t>
+  </si>
+  <si>
+    <t>milli</t>
+  </si>
+  <si>
+    <t>micro</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>nano</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>pico</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>femto</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>atto</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>zepto</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>yocto</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Short Prefix</t>
+  </si>
+  <si>
+    <t>Long Prefix</t>
+  </si>
+  <si>
+    <t>Magnitude</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>eV/molecule/K</t>
+  </si>
+  <si>
+    <t>kJ/K</t>
+  </si>
+  <si>
+    <t>eV/K</t>
+  </si>
+  <si>
+    <t>cal/K</t>
+  </si>
+  <si>
+    <t>kcal/K</t>
+  </si>
+  <si>
+    <t>Eh/K</t>
+  </si>
+  <si>
+    <t>Ha/K</t>
+  </si>
+  <si>
+    <t>cm/s</t>
+  </si>
+  <si>
+    <t>kPa</t>
+  </si>
+  <si>
+    <t>MPa</t>
+  </si>
+  <si>
+    <t>cm3/mol</t>
+  </si>
+  <si>
+    <t>mL/mol</t>
+  </si>
+  <si>
+    <t>L/mol</t>
+  </si>
+  <si>
+    <t>mJ</t>
   </si>
 </sst>
 </file>
@@ -790,74 +971,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -867,22 +986,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Input" xfId="1" builtinId="20" customBuiltin="1"/>
@@ -1200,13 +1309,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964A84F8-0654-4A01-81DA-CD635B4EF016}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,443 +1397,354 @@
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="e">
-        <f>R_JmolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C2" s="2" t="e">
-        <f>R_kJmolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D2" t="e">
-        <f>R_LPamol</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E2" s="2" t="e">
-        <f>R_cm3kPamolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F2" s="2" t="e">
-        <f>R_m3PamolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G2" t="e">
-        <f>R_cm3MPamolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H2" s="2" t="e">
-        <f>R_m3barmolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I2" s="2" t="e">
-        <f>R_LbarmolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J2" s="2" t="e">
-        <f>R_LtorrmolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K2" s="2" t="e">
-        <f>R_calmolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L2" s="2" t="e">
-        <f>R_kcalmolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M2" t="e">
-        <f>R_LatmmolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N2" t="e">
-        <f>R_cm3atmmolK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O2" s="2" t="e">
-        <f>R_eVK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P2" s="2" t="e">
-        <f>R_EhK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q2" s="2" t="e">
-        <f>R_HaK</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B2">
+        <f>INDEX(test_constants!$A$2:$A$6,ans!B1+1)</f>
+        <v>8.3144597999999998</v>
+      </c>
+      <c r="C2">
+        <f>INDEX(test_constants!$A$2:$A$6,ans!C1+1)</f>
+        <v>8.3144598E-3</v>
+      </c>
+      <c r="D2">
+        <f>INDEX(test_constants!$A$2:$A$6,ans!D1+1)</f>
+        <v>8.205733826794967E-2</v>
+      </c>
+      <c r="E2">
+        <f>INDEX(test_constants!$A$2:$A$6,ans!E1+1)</f>
+        <v>1.987203585086042E-3</v>
+      </c>
+      <c r="F2">
+        <f>INDEX(test_constants!$A$2:$A$6,ans!F1+1)</f>
+        <v>8.6173302692374234E-5</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="2" t="e">
-        <f>h_Js</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C3" s="2" t="e">
-        <f>h_kJs</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D3" s="2" t="e">
-        <f>h_eVs</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E3" s="2" t="e">
-        <f>h_Ehs</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F3" s="2" t="e">
-        <f>h_Has</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G3" s="2" t="e">
-        <f>h_Js/2/PI()</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H3" s="2" t="e">
-        <f>h_kJs/2/PI()</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I3" s="2" t="e">
-        <f>h_eVs/2/PI()</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J3" s="2" t="e">
-        <f>h_Ehs/2/PI()</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K3" s="2" t="e">
-        <f>h_Has/2/PI()</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B3" s="2">
+        <f>INDEX(test_constants!$A$9:$A$13,ans!B1+1)</f>
+        <v>6.6260700399999999E-34</v>
+      </c>
+      <c r="C3" s="2">
+        <f>INDEX(test_constants!$A$9:$A$13,ans!C1+1)</f>
+        <v>6.6260700399999995E-37</v>
+      </c>
+      <c r="D3" s="2">
+        <f>INDEX(test_constants!$A$9:$A$13,ans!D1+1)</f>
+        <v>4.1356676623401638E-15</v>
+      </c>
+      <c r="E3" s="2">
+        <f>INDEX(test_constants!$A$9:$A$13,ans!E1+1)</f>
+        <v>1.5198298208262026E-16</v>
+      </c>
+      <c r="F3" s="2">
+        <f>INDEX(test_constants!$A$9:$A$13,ans!F1+1)</f>
+        <v>1.5198298208262026E-16</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="2" t="e">
-        <f>kb_JK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C4" s="2" t="e">
-        <f>kb_kJK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D4" s="2" t="e">
-        <f>kb_eVK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E4" s="2" t="e">
-        <f>kb_calK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F4" s="2" t="e">
-        <f>kb_kcalK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G4" s="2" t="e">
-        <f>kb_EhK</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H4" s="2" t="e">
-        <f>kb_HaK</f>
-        <v>#REF!</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="B4" s="2">
+        <f>INDEX(test_constants!$A$16:$A$20,ans!B1+1)</f>
+        <v>1.0545718E-34</v>
+      </c>
+      <c r="C4" s="2">
+        <f>INDEX(test_constants!$A$16:$A$20,ans!C1+1)</f>
+        <v>1.0545718E-37</v>
+      </c>
+      <c r="D4" s="2">
+        <f>INDEX(test_constants!$A$16:$A$20,ans!D1+1)</f>
+        <v>6.5821195135991332E-16</v>
+      </c>
+      <c r="E4" s="2">
+        <f>INDEX(test_constants!$A$16:$A$20,ans!E1+1)</f>
+        <v>2.4188842861105135E-17</v>
+      </c>
+      <c r="F4" s="2">
+        <f>INDEX(test_constants!$A$16:$A$20,ans!F1+1)</f>
+        <v>2.4188842861105135E-17</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="e">
-        <f>c_ms</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C5" s="2" t="e">
-        <f>c_cms</f>
-        <v>#REF!</v>
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <f>INDEX(test_constants!$A$23:$A$29,B1+1)</f>
+        <v>1.3806485199999999E-23</v>
+      </c>
+      <c r="C5">
+        <f>INDEX(test_constants!$A$23:$A$29,C1+1)</f>
+        <v>1.3806485199999999E-26</v>
+      </c>
+      <c r="D5">
+        <f>INDEX(test_constants!$A$23:$A$29,D1+1)</f>
+        <v>8.6173303372172127E-5</v>
+      </c>
+      <c r="E5">
+        <f>INDEX(test_constants!$A$23:$A$29,E1+1)</f>
+        <v>3.2998291586998084E-24</v>
+      </c>
+      <c r="F5">
+        <f>INDEX(test_constants!$A$23:$A$29,F1+1)</f>
+        <v>3.2998291586998083E-27</v>
+      </c>
+      <c r="G5">
+        <f>INDEX(test_constants!$A$23:$A$29,G1+1)</f>
+        <v>3.1668104624737137E-6</v>
+      </c>
+      <c r="H5">
+        <f>INDEX(test_constants!$A$23:$A$29,H1+1)</f>
+        <v>3.1668104624737137E-6</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="2" t="e">
-        <f>m_e_kg</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C6" s="2" t="e">
-        <f>m_e_g</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D6" s="2" t="e">
-        <f>m_e_amu</f>
-        <v>#REF!</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B6" s="2">
+        <f>INDEX(test_constants!$A$32:$A$33,B1+1)</f>
+        <v>299792458</v>
+      </c>
+      <c r="C6" s="2">
+        <f>INDEX(test_constants!$A$32:$A$33,C1+1)</f>
+        <v>29979245800</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="2" t="e">
-        <f>m_p_kg</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C7" s="2" t="e">
-        <f>m_p_g</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D7" t="e">
-        <f>m_p_amu</f>
-        <v>#REF!</v>
+        <v>42</v>
+      </c>
+      <c r="B7" s="2">
+        <f>INDEX(test_constants!$A$36:$A$38,B1+1)</f>
+        <v>9.1093837015000008E-31</v>
+      </c>
+      <c r="C7" s="2">
+        <f>INDEX(test_constants!$A$36:$A$38,C1+1)</f>
+        <v>9.1093837015E-28</v>
+      </c>
+      <c r="D7" s="2">
+        <f>INDEX(test_constants!$A$36:$A$38,D1+1)</f>
+        <v>5.4856708650433128E-4</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="e">
-        <f>P0_bar</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C8" t="e">
-        <f>P0_atm</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D8" t="e">
-        <f>P0_Pa</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E8" t="e">
-        <f>P0_kPa</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F8" t="e">
-        <f>P0_MPa</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G8" t="e">
-        <f>P0_psi</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H8" t="e">
-        <f>P0_mmHg</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I8" t="e">
-        <f>P0_Torr</f>
-        <v>#REF!</v>
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <f>INDEX(test_constants!$A$41:$A$43,B1+1)</f>
+        <v>1.6726219236900001E-27</v>
+      </c>
+      <c r="C8">
+        <f>INDEX(test_constants!$A$41:$A$43,C1+1)</f>
+        <v>1.67262192369E-24</v>
+      </c>
+      <c r="D8">
+        <f>INDEX(test_constants!$A$41:$A$43,D1+1)</f>
+        <v>1.0072529224461204</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="e">
-        <f>T0_K</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" t="e">
-        <f>T0_C</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D9" t="e">
-        <f>T0_R</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E9" t="e">
-        <f>T0_F</f>
-        <v>#REF!</v>
+        <v>195</v>
+      </c>
+      <c r="B9">
+        <f>INDEX(test_constants!$A$46:$A$48,B1+1)</f>
+        <v>1.67492749804E-27</v>
+      </c>
+      <c r="C9">
+        <f>INDEX(test_constants!$A$46:$A$48,C1+1)</f>
+        <v>1.6749274980400001E-24</v>
+      </c>
+      <c r="D9">
+        <f>INDEX(test_constants!$A$46:$A$48,D1+1)</f>
+        <v>1.0086413393196902</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="e">
-        <f>V0_m3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C10" t="e">
-        <f>V0_cm3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D10" t="e">
-        <f>V0_ml</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E10" t="e">
-        <f>V0_L</f>
-        <v>#REF!</v>
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <f>INDEX(test_constants!$A$51:$A$58,B1+1)</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>INDEX(test_constants!$A$51:$A$58,C1+1)</f>
+        <v>0.98692326671601283</v>
+      </c>
+      <c r="D10">
+        <f>INDEX(test_constants!$A$51:$A$58,D1+1)</f>
+        <v>100000</v>
+      </c>
+      <c r="E10">
+        <f>INDEX(test_constants!$A$51:$A$58,E1+1)</f>
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <f>INDEX(test_constants!$A$51:$A$58,F1+1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="G10">
+        <f>INDEX(test_constants!$A$51:$A$58,G1+1)</f>
+        <v>14.50376807894691</v>
+      </c>
+      <c r="H10">
+        <f>INDEX(test_constants!$A$51:$A$58,H1+1)</f>
+        <v>750.06375541921057</v>
+      </c>
+      <c r="I10">
+        <f>INDEX(test_constants!$A$51:$A$58,I1+1)</f>
+        <v>750.06375541921057</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2">
-        <f>test_constants!A40</f>
+        <f>INDEX(test_constants!$A$61:$A$64,B1+1)</f>
         <v>298.14999999999998</v>
       </c>
-      <c r="C11">
-        <f>test_constants!A41</f>
+      <c r="C11" s="2">
+        <f>INDEX(test_constants!$A$61:$A$64,C1+1)</f>
         <v>25</v>
       </c>
-      <c r="D11">
-        <f>test_constants!A42</f>
-        <v>77</v>
-      </c>
-      <c r="E11">
-        <f>test_constants!A43</f>
-        <v>536.67000000000007</v>
-      </c>
-      <c r="F11">
-        <v>100</v>
+      <c r="D11" s="2">
+        <f>INDEX(test_constants!$A$61:$A$64,D1+1)</f>
+        <v>536.66999999999996</v>
+      </c>
+      <c r="E11" s="2">
+        <f>INDEX(test_constants!$A$61:$A$64,E1+1)</f>
+        <v>76.999999999999943</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="2" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
+        <v>46</v>
+      </c>
+      <c r="B12" s="2">
+        <f>INDEX(test_constants!$A$67:$A$70,B1+1)</f>
+        <v>2.47895618936999E-2</v>
+      </c>
+      <c r="C12" s="2">
+        <f>INDEX(test_constants!$A$67:$A$70,C1+1)</f>
+        <v>24789.561893699898</v>
+      </c>
+      <c r="D12" s="2">
+        <f>INDEX(test_constants!$A$67:$A$70,D1+1)</f>
+        <v>24789.561893699902</v>
+      </c>
+      <c r="E12" s="2">
+        <f>INDEX(test_constants!$A$67:$A$70,E1+1)</f>
+        <v>24.789561893699901</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="2" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
+        <v>196</v>
+      </c>
+      <c r="B13" s="2">
+        <f>test_constants!A73</f>
+        <v>6.0221408599999999E+23</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="2" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
+        <v>197</v>
+      </c>
+      <c r="B14" s="2">
+        <f>test_constants!A76</f>
+        <v>6.0221408599999999E+23</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="2" t="e">
-        <f>test_constants!#REF!*constants!#REF!/constants!#REF!</f>
-        <v>#REF!</v>
+        <v>198</v>
+      </c>
+      <c r="B15" s="2">
+        <f>test_constants!A79</f>
+        <v>1.6021766208000001E-19</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="2" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="B16" s="2">
+        <f>test_constants!A82</f>
+        <v>96485.332930564007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="2" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="B17" s="2">
+        <f>test_constants!A85</f>
+        <v>6.6742999999999994E-11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="B18" s="2">
+        <f>test_constants!A88</f>
+        <v>8.8541878128000006E-12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="B19">
+        <f>test_constants!A91</f>
+        <v>1.2566370621199999E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="B20">
+        <f>INDEX(test_constants!$A$94:$A$95,B1+1)</f>
+        <v>2.1799233153862099E-18</v>
+      </c>
+      <c r="C20">
+        <f>INDEX(test_constants!$A$94:$A$95,C1+1)</f>
+        <v>2.1799233153862101E-15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" t="e">
-        <f>test_constants!#REF!</f>
-        <v>#REF!</v>
+        <v>204</v>
+      </c>
+      <c r="B21">
+        <f>test_constants!A98</f>
+        <v>5.2916483301109397E-11</v>
       </c>
     </row>
   </sheetData>
@@ -1731,10 +1754,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E805CA-ACAA-4599-A8B2-1C6F37F3FD7A}">
-  <dimension ref="A29:B47"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B99"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="1">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,135 +1771,689 @@
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <f>R_</f>
+        <v>8.3144597999999998</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <f>R_/kilo_</f>
+        <v>8.3144598E-3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f>R_/Units!B88</f>
+        <v>8.205733826794967E-2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <f>R_/Units!B86/kilo_</f>
+        <v>1.987203585086042E-3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <f>R_/Units!B87/N0_</f>
+        <v>8.6173302692374234E-5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f>h_</f>
+        <v>6.6260700399999999E-34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f>h_/kilo_</f>
+        <v>6.6260700399999995E-37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <f>h_/Units!B87</f>
+        <v>4.1356676623401638E-15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f>h_/Units!B89</f>
+        <v>1.5198298208262026E-16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f>h_/Units!B90</f>
+        <v>1.5198298208262026E-16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f>h_bar_</f>
+        <v>1.0545718E-34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <f>h_bar_/kilo_</f>
+        <v>1.0545718E-37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <f>h_bar_/Units!B87</f>
+        <v>6.5821195135991332E-16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <f>h_bar_/Units!B89</f>
+        <v>2.4188842861105135E-17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f>h_bar_/Units!B89</f>
+        <v>2.4188842861105135E-17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f>kb_</f>
+        <v>1.3806485199999999E-23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f>kb_/kilo_</f>
+        <v>1.3806485199999999E-26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <f>kb_/Units!B87</f>
+        <v>8.6173303372172127E-5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <f>kb_/Units!B86</f>
+        <v>3.2998291586998084E-24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <f>kb_/Units!B86/kilo_</f>
+        <v>3.2998291586998083E-27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <f>kb_/Units!B89</f>
+        <v>3.1668104624737137E-6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <f>kb_/Units!B90</f>
+        <v>3.1668104624737137E-6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <f>c_</f>
+        <v>299792458</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <f>c_/centI_</f>
+        <v>29979245800</v>
+      </c>
+      <c r="B33" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <f>m_e_</f>
+        <v>9.1093837015000008E-31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <f>m_e_*kilo_</f>
+        <v>9.1093837015E-28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <f>m_e_/Units!B30</f>
+        <v>5.4856708650433128E-4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <f>m_p_</f>
+        <v>1.6726219236900001E-27</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <f>m_p_*kilo_</f>
+        <v>1.67262192369E-24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <f>m_p_/Units!B30</f>
+        <v>1.0072529224461204</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <f>m_n_</f>
+        <v>1.67492749804E-27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <f>m_n_*kilo_</f>
+        <v>1.6749274980400001E-24</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <f>m_n_/Units!B30</f>
+        <v>1.0086413393196902</v>
+      </c>
+      <c r="B48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <f>P0_/Units!B99</f>
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <f>P0_/Units!B98</f>
+        <v>0.98692326671601283</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <f>P0_</f>
+        <v>100000</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <f>P0_/kilo_</f>
+        <v>100</v>
+      </c>
+      <c r="B54" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <f>P0_/mega_</f>
+        <v>0.1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <f>P0_/Units!B103</f>
+        <v>14.50376807894691</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <f>P0_/Units!B100</f>
+        <v>750.06375541921057</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <f>P0_/Units!B102</f>
+        <v>750.06375541921057</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <f>T0_</f>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <f>A61-273.15</f>
+        <v>25</v>
+      </c>
+      <c r="B62" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <f>A61*9/5</f>
+        <v>536.66999999999996</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <f>A63-459.67</f>
+        <v>76.999999999999943</v>
+      </c>
+      <c r="B64" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="6"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="e">
-        <f>h_Js/2/PI()</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="e">
-        <f>h_kJs/2/PI()</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="e">
-        <f>h_eVs/2/PI()</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="e">
-        <f>h_Ehs/2/PI()</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14" t="e">
-        <f>h_Has/2/PI()</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
-        <v>298.14999999999998</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="12">
-        <f>A40-273.15</f>
-        <v>25</v>
-      </c>
-      <c r="B41" s="6" t="s">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <f>V0_</f>
+        <v>2.47895618936999E-2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <f>V0_/centI_^3</f>
+        <v>24789.561893699898</v>
+      </c>
+      <c r="B68" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <f>V0_/Units!B67/milli_</f>
+        <v>24789.561893699902</v>
+      </c>
+      <c r="B69" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <f>V0_/Units!B67</f>
+        <v>24.789561893699901</v>
+      </c>
+      <c r="B70" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <f>N0_</f>
+        <v>6.0221408599999999E+23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <f>Na_</f>
+        <v>6.0221408599999999E+23</v>
+      </c>
+      <c r="B76" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <f>e_</f>
+        <v>1.6021766208000001E-19</v>
+      </c>
+      <c r="B79" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
-        <f>(A41*9/5)+32</f>
-        <v>77</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="12">
-        <f>A42+459.67</f>
-        <v>536.67000000000007</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="6"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14">
-        <f>1/6242000000000000000</f>
-        <v>1.6020506247997438E-19</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>69</v>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <f>F_</f>
+        <v>96485.332930564007</v>
+      </c>
+      <c r="B82" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <f>G_</f>
+        <v>6.6742999999999994E-11</v>
+      </c>
+      <c r="B85" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <f>eps_0_</f>
+        <v>8.8541878128000006E-12</v>
+      </c>
+      <c r="B88" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <f>mu_0_</f>
+        <v>1.2566370621199999E-6</v>
+      </c>
+      <c r="B91" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <f>R_inf_</f>
+        <v>2.1799233153862099E-18</v>
+      </c>
+      <c r="B94" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <f>R_inf_/milli_</f>
+        <v>2.1799233153862101E-15</v>
+      </c>
+      <c r="B95" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <f>r_bohr_</f>
+        <v>5.2916483301109397E-11</v>
+      </c>
+      <c r="B98" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1886,11 +2466,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2E394F-E007-4BF1-81D0-B5B598FFC5B9}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,10 +2492,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,7 +2503,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="C2">
         <v>8.3144597999999998</v>
@@ -1945,10 +2528,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C4">
         <v>1.0545718E-34</v>
@@ -1990,7 +2573,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="C7">
         <v>9.1093837015000008E-31</v>
@@ -2004,7 +2587,7 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="C8">
         <v>1.6726219236900001E-27</v>
@@ -2015,10 +2598,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="C9">
         <v>1.67492749804E-27</v>
@@ -2032,7 +2615,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C10">
         <v>100000</v>
@@ -2046,7 +2629,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="C11">
         <v>298.14999999999998</v>
@@ -2060,21 +2643,21 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="C12">
         <v>2.47895618936999E-2</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C13">
         <v>6.0221408599999999E+23</v>
@@ -2085,13 +2668,13 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="C14">
         <v>6.0221408599999999E+23</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2099,7 +2682,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="C15">
         <v>1.6021766208000001E-19</v>
@@ -2113,83 +2696,83 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="C16">
         <v>96485.332930564007</v>
       </c>
       <c r="D16" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="C17">
         <v>6.6742999999999994E-11</v>
       </c>
       <c r="D17" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="C18">
         <v>8.8541878128000006E-12</v>
       </c>
       <c r="D18" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B19" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="C19">
         <v>1.2566370621199999E-6</v>
       </c>
       <c r="D19" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="B20" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C20">
         <v>2.1799233153862099E-18</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="C21">
         <v>5.2916483301109397E-11</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2200,10 +2783,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C94EC0A-8D3A-4151-9597-FE396F0E5C3A}">
-  <dimension ref="A2:C147"/>
+  <dimension ref="A2:C170"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
+    </sheetView>
+    <sheetView topLeftCell="A82" workbookViewId="1">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,73 +2801,73 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B8">
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2292,144 +2878,144 @@
         <v>3600</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B10">
         <v>3600</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B11">
         <v>3600</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>86400</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B13">
         <v>604800</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>31557600</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>31557600</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B21" s="2">
         <v>1.6605390395999399E-24</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B22" s="2">
         <v>1.6605390395999399E-24</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B23" s="2">
         <v>1.6605390395999399E-24</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2437,19 +3023,19 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2460,29 +3046,29 @@
         <v>1E-3</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B28">
         <v>1E-3</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="B29" s="2">
         <v>1.66057788110262E-27</v>
       </c>
       <c r="C29" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2493,166 +3079,166 @@
         <v>1.66057788110262E-27</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="B31" s="2">
         <v>1.66057788110262E-27</v>
       </c>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B32" s="2">
         <v>1.66057788110262E-27</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B33">
         <v>0.45359290943563901</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="B34">
         <v>0.45359290943563901</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="B40">
         <v>2.53999862840074E-2</v>
       </c>
       <c r="C40" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B41">
         <v>2.53999862840074E-2</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="B42">
         <v>0.30479999024639998</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B43">
         <v>0.30479999024639998</v>
       </c>
       <c r="C43" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B44">
         <v>0.30479999024639998</v>
       </c>
       <c r="C44" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B45">
         <v>1609.3440000000001</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="B46" s="2">
         <v>1E-10</v>
       </c>
       <c r="C46" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2660,19 +3246,19 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2683,18 +3269,18 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2705,110 +3291,110 @@
         <v>1.8</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="B53">
         <v>1.8</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2819,247 +3405,247 @@
         <v>1E-3</v>
       </c>
       <c r="C67" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B68">
         <v>1E-3</v>
       </c>
       <c r="C68" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B72">
         <v>9.8066499999999994</v>
       </c>
       <c r="C72" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B78" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C78" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B79" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C79" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B80">
         <v>4.4482220000000003</v>
       </c>
       <c r="C80" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B84">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B85">
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B86">
         <v>4.1840000000000002</v>
       </c>
       <c r="C86" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>65</v>
-      </c>
-      <c r="B87" s="2">
+        <v>48</v>
+      </c>
+      <c r="B87">
         <v>1.6021766208000001E-19</v>
       </c>
       <c r="C87" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B88">
         <v>101.325</v>
       </c>
       <c r="C88" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B89" s="2">
         <v>4.3597447222071E-18</v>
       </c>
       <c r="C89" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B90" s="2">
         <v>4.3597447222071E-18</v>
       </c>
       <c r="C90" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="B91" s="2">
         <v>4.3597447222071E-18</v>
       </c>
       <c r="C91" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="B92">
         <v>1055</v>
       </c>
       <c r="C92" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3070,18 +3656,18 @@
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="B97">
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3092,7 +3678,7 @@
         <v>101325</v>
       </c>
       <c r="C98" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3103,7 +3689,7 @@
         <v>100000</v>
       </c>
       <c r="C99" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3114,18 +3700,18 @@
         <v>133.322</v>
       </c>
       <c r="C100" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="B101">
         <v>133.322</v>
       </c>
       <c r="C101" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3136,7 +3722,7 @@
         <v>133.322</v>
       </c>
       <c r="C102" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -3147,23 +3733,23 @@
         <v>6894.76</v>
       </c>
       <c r="C103" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3174,110 +3760,110 @@
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B108">
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="B113">
         <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="B118">
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3288,34 +3874,34 @@
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="B123">
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3326,159 +3912,395 @@
         <v>1</v>
       </c>
       <c r="C127" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B128">
         <v>1</v>
       </c>
       <c r="C128" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B132">
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B137">
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="B141">
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B142">
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="B146">
         <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="B147">
         <v>1</v>
       </c>
       <c r="C147" t="s">
-        <v>164</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>208</v>
+      </c>
+      <c r="B151" t="s">
+        <v>209</v>
+      </c>
+      <c r="C151" s="2">
+        <v>9.9999999999999998E+23</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>210</v>
+      </c>
+      <c r="B152" t="s">
+        <v>211</v>
+      </c>
+      <c r="C152" s="2">
+        <v>1E+21</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>212</v>
+      </c>
+      <c r="B153" t="s">
+        <v>213</v>
+      </c>
+      <c r="C153" s="2">
+        <v>1E+18</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>214</v>
+      </c>
+      <c r="B154" t="s">
+        <v>215</v>
+      </c>
+      <c r="C154" s="2">
+        <v>1000000000000000</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>216</v>
+      </c>
+      <c r="B155" t="s">
+        <v>119</v>
+      </c>
+      <c r="C155" s="2">
+        <v>1000000000000</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>217</v>
+      </c>
+      <c r="B156" t="s">
+        <v>181</v>
+      </c>
+      <c r="C156" s="2">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>218</v>
+      </c>
+      <c r="B157" t="s">
+        <v>219</v>
+      </c>
+      <c r="C157" s="2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>220</v>
+      </c>
+      <c r="B158" t="s">
+        <v>221</v>
+      </c>
+      <c r="C158" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>222</v>
+      </c>
+      <c r="B159" t="s">
+        <v>23</v>
+      </c>
+      <c r="C159" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>223</v>
+      </c>
+      <c r="B160" t="s">
+        <v>224</v>
+      </c>
+      <c r="C160" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>225</v>
+      </c>
+      <c r="B161" t="s">
+        <v>226</v>
+      </c>
+      <c r="C161" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>227</v>
+      </c>
+      <c r="B162" t="s">
+        <v>19</v>
+      </c>
+      <c r="C162" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>228</v>
+      </c>
+      <c r="B163" t="s">
+        <v>66</v>
+      </c>
+      <c r="C163" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>229</v>
+      </c>
+      <c r="B164" t="s">
+        <v>230</v>
+      </c>
+      <c r="C164" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>231</v>
+      </c>
+      <c r="B165" t="s">
+        <v>232</v>
+      </c>
+      <c r="C165" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>233</v>
+      </c>
+      <c r="B166" t="s">
+        <v>234</v>
+      </c>
+      <c r="C166" s="2">
+        <v>9.9999999999999998E-13</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>235</v>
+      </c>
+      <c r="B167" t="s">
+        <v>236</v>
+      </c>
+      <c r="C167" s="2">
+        <v>1.0000000000000001E-15</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>237</v>
+      </c>
+      <c r="B168" t="s">
+        <v>238</v>
+      </c>
+      <c r="C168" s="2">
+        <v>1.0000000000000001E-18</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>239</v>
+      </c>
+      <c r="B169" t="s">
+        <v>240</v>
+      </c>
+      <c r="C169" s="2">
+        <v>9.9999999999999991E-22</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>241</v>
+      </c>
+      <c r="B170" t="s">
+        <v>242</v>
+      </c>
+      <c r="C170" s="2">
+        <v>9.9999999999999992E-25</v>
       </c>
     </row>
   </sheetData>
@@ -3492,6 +4314,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>